<commit_message>
Tax Doc Update 20260113
</commit_message>
<xml_diff>
--- a/A/TaxPrep/BusinessWorksheet.xlsx
+++ b/A/TaxPrep/BusinessWorksheet.xlsx
@@ -14,7 +14,7 @@
     <sheet name="AssetPurchases" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">BusinessMileage!$A$1:$B$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">BusinessMileage!$A$1:$B$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">HomeOffice!$A$1:$C$29</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
   <si>
     <t>Income</t>
   </si>
@@ -323,9 +323,6 @@
   </si>
   <si>
     <t>Gross Receipts non included above</t>
-  </si>
-  <si>
-    <t>Business Miles Driven (1/1 - 6/30)</t>
   </si>
   <si>
     <t>Total Miles Driven w/ this vehicle (all purposes 1/1-12/31)</t>
@@ -723,8 +720,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>789878</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>23231</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -733,8 +730,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8154329" y="290396"/>
-          <a:ext cx="3995854" cy="5076128"/>
+          <a:off x="6493262" y="290396"/>
+          <a:ext cx="3995854" cy="5052897"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1633,7 +1630,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1675,7 +1672,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="14"/>
@@ -1684,7 +1681,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="14"/>
@@ -1693,43 +1690,44 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="27"/>
+        <v>51</v>
+      </c>
+      <c r="B6" s="28"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="28"/>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="29"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="29"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="25"/>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="25"/>
+      <c r="A10" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="26"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="26"/>
+        <v>56</v>
+      </c>
+      <c r="B11" s="27"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -1739,113 +1737,89 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="29"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="25"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="26"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="27"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="28"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="29"/>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="27"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="26"/>
+        <v>96</v>
+      </c>
+      <c r="B19" s="27"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="28"/>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="29"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="25"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="26"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="27"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="27"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="27"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="27"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="28"/>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="29"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="25"/>
+      <c r="B26" s="27"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="26"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="27"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="27"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" s="27"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="28"/>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="B27" s="28"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B28" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>